<commit_message>
load data on web
load data from web in market_data lab
</commit_message>
<xml_diff>
--- a/Modeling/yeast_data.xlsx
+++ b/Modeling/yeast_data.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\SVGS-FP\Staff\tylera\Documents\MATLAB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tylera\OneDrive - Shenandoah Valley Governor's School\Math Modeling\My Course\2 - Discrete Dynamic Systems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4DEAC7-F83E-4F35-9AED-791943077456}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{FE4DEAC7-F83E-4F35-9AED-791943077456}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{C5527BAD-7F12-486C-A6D4-32B9FED59CE6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{FD317C29-E6EC-4602-8A8D-58EA56749EA7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{FD317C29-E6EC-4602-8A8D-58EA56749EA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>day</t>
   </si>
@@ -34,6 +35,15 @@
   </si>
   <si>
     <t>change_in_biomass</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>digoxin</t>
+  </si>
+  <si>
+    <t>change_digoxin</t>
   </si>
 </sst>
 </file>
@@ -387,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{427FA910-D783-4CA1-87A7-9C8712C49FB7}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,4 +641,126 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{405CE188-8664-4988-8F83-48D156B76F7F}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+      <c r="C2">
+        <v>-0.155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="C3">
+        <v>-0.107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="C4">
+        <v>-7.3999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="C5">
+        <v>-5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.113</v>
+      </c>
+      <c r="C6">
+        <v>-3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>7.8E-2</v>
+      </c>
+      <c r="C7">
+        <v>-2.4E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="C8">
+        <v>-1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="C9">
+        <v>-1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>